<commit_message>
add employee api tests
</commit_message>
<xml_diff>
--- a/resources/xlsData/Sample.xlsx
+++ b/resources/xlsData/Sample.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DN137\git\tasom-multifonds\Main-Development-Branch\resources\xlsData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28E370F-F309-4A75-A778-CAA4908BA8E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{88098AA0-C9B2-4081-9AFC-2AF33F8748CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1275" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sample.Items" sheetId="1" r:id="rId1"/>
+    <sheet name="Sample.Employees" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,39 +21,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>itemId</t>
-  </si>
-  <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>propertyName</t>
   </si>
   <si>
-    <t>Sausage</t>
-  </si>
-  <si>
-    <t>BBQ time</t>
-  </si>
-  <si>
-    <t>Flippers</t>
-  </si>
-  <si>
-    <t>Summer time</t>
-  </si>
-  <si>
-    <t>item-1</t>
-  </si>
-  <si>
-    <t>item-2</t>
-  </si>
-  <si>
-    <t>price</t>
+    <t>employee_age</t>
+  </si>
+  <si>
+    <t>employee-1</t>
+  </si>
+  <si>
+    <t>employee-2</t>
+  </si>
+  <si>
+    <t>Miss Piggy</t>
+  </si>
+  <si>
+    <t>Kermet Frog</t>
+  </si>
+  <si>
+    <t>employee_name</t>
+  </si>
+  <si>
+    <t>employee_salary</t>
   </si>
 </sst>
 </file>
@@ -67,7 +54,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$€-2]\ #,##0.00;[Red]\-[$€-2]\ #,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +73,12 @@
     <font>
       <sz val="11"/>
       <color theme="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -402,77 +395,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:E7"/>
+  <dimension ref="B3:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C3" sqref="C3:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="4" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4</v>
       </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="C5" s="1">
+        <v>50000</v>
+      </c>
+      <c r="D5" s="1">
+        <v>45000</v>
+      </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0.89</v>
-      </c>
-      <c r="D6" s="1">
-        <v>19.989999999999998</v>
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>33</v>
+      </c>
+      <c r="D6">
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
+      <c r="B7" s="2"/>
     </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
   <headerFooter>

</xml_diff>